<commit_message>
Update: improved Excel stacked chart export logic
</commit_message>
<xml_diff>
--- a/data/hackathon_dashboard_output.xlsx
+++ b/data/hackathon_dashboard_output.xlsx
@@ -14,13 +14,15 @@
     <sheet name="Weekday Revenue" sheetId="5" r:id="rId5"/>
     <sheet name="Merchant Revenue" sheetId="6" r:id="rId6"/>
     <sheet name="Age Revenue" sheetId="7" r:id="rId7"/>
+    <sheet name="Stacked Merchant Revenue" sheetId="8" r:id="rId8"/>
+    <sheet name="Stacked Age Revenue" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="38">
   <si>
     <t>Month</t>
   </si>
@@ -134,12 +136,6 @@
   </si>
   <si>
     <t>unknown</t>
-  </si>
-  <si>
-    <t>Tip: Pivot this in Excel for stacked view</t>
-  </si>
-  <si>
-    <t>Tip: Use Excel PivotChart for Age breakdown</t>
   </si>
 </sst>
 </file>
@@ -1219,6 +1215,1366 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50050001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Stacked Revenue by Merchant</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked Merchant Revenue'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gmobile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Stacked Merchant Revenue'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2020-01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020-02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020-03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020-04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020-05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2020-06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020-07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020-08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020-09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2020-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020-11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2020-12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stacked Merchant Revenue'!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked Merchant Revenue'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mobifone</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Stacked Merchant Revenue'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2020-01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020-02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020-03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020-04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020-05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2020-06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020-07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020-08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020-09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2020-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020-11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2020-12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stacked Merchant Revenue'!$C$2:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>456427.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>407100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>513600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>424500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>465000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>539400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>459000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>464700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>417600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>543300</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>459300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>570600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked Merchant Revenue'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vietnamobile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Stacked Merchant Revenue'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2020-01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020-02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020-03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020-04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020-05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2020-06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020-07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020-08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020-09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2020-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020-11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2020-12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stacked Merchant Revenue'!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>45600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>79200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>62000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>106400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>62800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>86400</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>137200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked Merchant Revenue'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Viettel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Stacked Merchant Revenue'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2020-01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020-02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020-03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020-04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020-05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2020-06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020-07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020-08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020-09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2020-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020-11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2020-12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stacked Merchant Revenue'!$E$2:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>591200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>593400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>572800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>537200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>501400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>536200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>624400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>627000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>550800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>599800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>679400</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>687800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked Merchant Revenue'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vinaphone</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Stacked Merchant Revenue'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2020-01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020-02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020-03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020-04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020-05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2020-06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020-07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020-08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020-09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2020-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020-11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2020-12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stacked Merchant Revenue'!$F$2:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>317200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>348000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>438400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>480800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>421200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>488800</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>424800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>422400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>361600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>489200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>315200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>368800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:overlap val="100"/>
+        <c:axId val="50060001"/>
+        <c:axId val="50060002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50060001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Month</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50060002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50060002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Revenue (VND)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50060001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Stacked Revenue by Age Group</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked Age Revenue'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>18_to_22</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Stacked Age Revenue'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2020-01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020-02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020-03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020-04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020-05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2020-06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020-07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020-08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020-09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2020-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020-11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2020-12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stacked Age Revenue'!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>98500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>111100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>132300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>149200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>123400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>129000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>119600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>104300</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>148900</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>141300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>169800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked Age Revenue'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>23_to_27</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Stacked Age Revenue'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2020-01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020-02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020-03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020-04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020-05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2020-06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020-07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020-08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020-09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2020-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020-11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2020-12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stacked Age Revenue'!$C$2:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>380300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>369200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>426800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>344400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>366900</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>342700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>370800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>419000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>367400</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>324400</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>297200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>406900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked Age Revenue'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>28_to_32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Stacked Age Revenue'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2020-01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020-02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020-03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020-04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020-05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2020-06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020-07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020-08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020-09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2020-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020-11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2020-12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stacked Age Revenue'!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>338900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>350600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>395000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>303600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>335400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>412400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>371800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>343700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>284100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>308900</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>258100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>333800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked Age Revenue'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>33_to_37</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Stacked Age Revenue'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2020-01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020-02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020-03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020-04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020-05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2020-06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020-07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020-08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020-09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2020-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020-11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2020-12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stacked Age Revenue'!$E$2:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>199427.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>183200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>185200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>267500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>229300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>179600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>258900</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>219300</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>317800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>249600</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>314700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked Age Revenue'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>&gt;37</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Stacked Age Revenue'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2020-01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020-02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020-03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020-04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020-05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2020-06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020-07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020-08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020-09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2020-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020-11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2020-12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stacked Age Revenue'!$F$2:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>128600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>154600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>148800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>145600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>161300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>239300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>224800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>168300</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>171700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>266300</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>236300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>179900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stacked Age Revenue'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>unknown</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Stacked Age Revenue'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2020-01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020-02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020-03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020-04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020-05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2020-06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020-07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020-08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020-09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2020-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020-11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2020-12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stacked Age Revenue'!$G$2:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>264700</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>212200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>297900</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>279000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>229200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>273700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>286300</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>311800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>246400</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>336800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>357800</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>359300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:overlap val="100"/>
+        <c:axId val="50070001"/>
+        <c:axId val="50070002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50070001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Month</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50070002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50070002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Revenue (VND)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50070001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1388,6 +2744,76 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -2247,13 +3673,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2263,11 +3689,8 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2278,7 +3701,7 @@
         <v>456427.02</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2289,7 +3712,7 @@
         <v>45600</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2300,7 +3723,7 @@
         <v>591200</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2311,7 +3734,7 @@
         <v>317200</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2322,7 +3745,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2333,7 +3756,7 @@
         <v>407100</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2344,7 +3767,7 @@
         <v>30400</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -2355,7 +3778,7 @@
         <v>593400</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -2366,7 +3789,7 @@
         <v>348000</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2377,7 +3800,7 @@
         <v>513600</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2388,7 +3811,7 @@
         <v>61200</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -2399,7 +3822,7 @@
         <v>572800</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2410,7 +3833,7 @@
         <v>438400</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -2421,7 +3844,7 @@
         <v>424500</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -2835,13 +4258,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2851,11 +4274,8 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2866,7 +4286,7 @@
         <v>98500</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2877,7 +4297,7 @@
         <v>380300</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2888,7 +4308,7 @@
         <v>338900</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2899,7 +4319,7 @@
         <v>199427.02</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2910,7 +4330,7 @@
         <v>128600</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2921,7 +4341,7 @@
         <v>264700</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2932,7 +4352,7 @@
         <v>111100</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -2943,7 +4363,7 @@
         <v>369200</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -2954,7 +4374,7 @@
         <v>350600</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -2965,7 +4385,7 @@
         <v>183200</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -2976,7 +4396,7 @@
         <v>154600</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -2987,7 +4407,7 @@
         <v>212200</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2998,7 +4418,7 @@
         <v>132300</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -3009,7 +4429,7 @@
         <v>426800</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -3650,4 +5070,591 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>456427.02</v>
+      </c>
+      <c r="D2">
+        <v>45600</v>
+      </c>
+      <c r="E2">
+        <v>591200</v>
+      </c>
+      <c r="F2">
+        <v>317200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2000</v>
+      </c>
+      <c r="C3">
+        <v>407100</v>
+      </c>
+      <c r="D3">
+        <v>30400</v>
+      </c>
+      <c r="E3">
+        <v>593400</v>
+      </c>
+      <c r="F3">
+        <v>348000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>513600</v>
+      </c>
+      <c r="D4">
+        <v>61200</v>
+      </c>
+      <c r="E4">
+        <v>572800</v>
+      </c>
+      <c r="F4">
+        <v>438400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>424500</v>
+      </c>
+      <c r="D5">
+        <v>46800</v>
+      </c>
+      <c r="E5">
+        <v>537200</v>
+      </c>
+      <c r="F5">
+        <v>480800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>465000</v>
+      </c>
+      <c r="D6">
+        <v>79200</v>
+      </c>
+      <c r="E6">
+        <v>501400</v>
+      </c>
+      <c r="F6">
+        <v>421200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>539400</v>
+      </c>
+      <c r="D7">
+        <v>62000</v>
+      </c>
+      <c r="E7">
+        <v>536200</v>
+      </c>
+      <c r="F7">
+        <v>488800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>459000</v>
+      </c>
+      <c r="D8">
+        <v>75600</v>
+      </c>
+      <c r="E8">
+        <v>624400</v>
+      </c>
+      <c r="F8">
+        <v>424800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>800</v>
+      </c>
+      <c r="C9">
+        <v>464700</v>
+      </c>
+      <c r="D9">
+        <v>106400</v>
+      </c>
+      <c r="E9">
+        <v>627000</v>
+      </c>
+      <c r="F9">
+        <v>422400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>400</v>
+      </c>
+      <c r="C10">
+        <v>417600</v>
+      </c>
+      <c r="D10">
+        <v>62800</v>
+      </c>
+      <c r="E10">
+        <v>550800</v>
+      </c>
+      <c r="F10">
+        <v>361600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>543300</v>
+      </c>
+      <c r="D11">
+        <v>70800</v>
+      </c>
+      <c r="E11">
+        <v>599800</v>
+      </c>
+      <c r="F11">
+        <v>489200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>459300</v>
+      </c>
+      <c r="D12">
+        <v>86400</v>
+      </c>
+      <c r="E12">
+        <v>679400</v>
+      </c>
+      <c r="F12">
+        <v>315200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>570600</v>
+      </c>
+      <c r="D13">
+        <v>137200</v>
+      </c>
+      <c r="E13">
+        <v>687800</v>
+      </c>
+      <c r="F13">
+        <v>368800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>98500</v>
+      </c>
+      <c r="C2">
+        <v>380300</v>
+      </c>
+      <c r="D2">
+        <v>338900</v>
+      </c>
+      <c r="E2">
+        <v>199427.02</v>
+      </c>
+      <c r="F2">
+        <v>128600</v>
+      </c>
+      <c r="G2">
+        <v>264700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>111100</v>
+      </c>
+      <c r="C3">
+        <v>369200</v>
+      </c>
+      <c r="D3">
+        <v>350600</v>
+      </c>
+      <c r="E3">
+        <v>183200</v>
+      </c>
+      <c r="F3">
+        <v>154600</v>
+      </c>
+      <c r="G3">
+        <v>212200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>132300</v>
+      </c>
+      <c r="C4">
+        <v>426800</v>
+      </c>
+      <c r="D4">
+        <v>395000</v>
+      </c>
+      <c r="E4">
+        <v>185200</v>
+      </c>
+      <c r="F4">
+        <v>148800</v>
+      </c>
+      <c r="G4">
+        <v>297900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>149200</v>
+      </c>
+      <c r="C5">
+        <v>344400</v>
+      </c>
+      <c r="D5">
+        <v>303600</v>
+      </c>
+      <c r="E5">
+        <v>267500</v>
+      </c>
+      <c r="F5">
+        <v>145600</v>
+      </c>
+      <c r="G5">
+        <v>279000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>123400</v>
+      </c>
+      <c r="C6">
+        <v>366900</v>
+      </c>
+      <c r="D6">
+        <v>335400</v>
+      </c>
+      <c r="E6">
+        <v>250600</v>
+      </c>
+      <c r="F6">
+        <v>161300</v>
+      </c>
+      <c r="G6">
+        <v>229200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>129000</v>
+      </c>
+      <c r="C7">
+        <v>342700</v>
+      </c>
+      <c r="D7">
+        <v>412400</v>
+      </c>
+      <c r="E7">
+        <v>229300</v>
+      </c>
+      <c r="F7">
+        <v>239300</v>
+      </c>
+      <c r="G7">
+        <v>273700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>150500</v>
+      </c>
+      <c r="C8">
+        <v>370800</v>
+      </c>
+      <c r="D8">
+        <v>371800</v>
+      </c>
+      <c r="E8">
+        <v>179600</v>
+      </c>
+      <c r="F8">
+        <v>224800</v>
+      </c>
+      <c r="G8">
+        <v>286300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>119600</v>
+      </c>
+      <c r="C9">
+        <v>419000</v>
+      </c>
+      <c r="D9">
+        <v>343700</v>
+      </c>
+      <c r="E9">
+        <v>258900</v>
+      </c>
+      <c r="F9">
+        <v>168300</v>
+      </c>
+      <c r="G9">
+        <v>311800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>104300</v>
+      </c>
+      <c r="C10">
+        <v>367400</v>
+      </c>
+      <c r="D10">
+        <v>284100</v>
+      </c>
+      <c r="E10">
+        <v>219300</v>
+      </c>
+      <c r="F10">
+        <v>171700</v>
+      </c>
+      <c r="G10">
+        <v>246400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>148900</v>
+      </c>
+      <c r="C11">
+        <v>324400</v>
+      </c>
+      <c r="D11">
+        <v>308900</v>
+      </c>
+      <c r="E11">
+        <v>317800</v>
+      </c>
+      <c r="F11">
+        <v>266300</v>
+      </c>
+      <c r="G11">
+        <v>336800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>141300</v>
+      </c>
+      <c r="C12">
+        <v>297200</v>
+      </c>
+      <c r="D12">
+        <v>258100</v>
+      </c>
+      <c r="E12">
+        <v>249600</v>
+      </c>
+      <c r="F12">
+        <v>236300</v>
+      </c>
+      <c r="G12">
+        <v>357800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>169800</v>
+      </c>
+      <c r="C13">
+        <v>406900</v>
+      </c>
+      <c r="D13">
+        <v>333800</v>
+      </c>
+      <c r="E13">
+        <v>314700</v>
+      </c>
+      <c r="F13">
+        <v>179900</v>
+      </c>
+      <c r="G13">
+        <v>359300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>